<commit_message>
add rabbitmq for update data
</commit_message>
<xml_diff>
--- a/fileUpload/report.xlsx
+++ b/fileUpload/report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\python\flask\Flask-SQLAlchemy-Postgre-sendEmail-exportExcel-crobjob-rabbitmq-redisCache-pusher\fileUpload\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC24ACAC-34FF-43E9-9288-1F13B7493B9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512051BE-5211-40C1-91E1-E61898B06012}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Email: </t>
   </si>
@@ -49,10 +49,7 @@
     <t>1020211201202</t>
   </si>
   <si>
-    <t>mxcxcxc@yahoo.com</t>
-  </si>
-  <si>
-    <t>ajjkjk@yahoo.com</t>
+    <t>acacacax21@yahoo.com</t>
   </si>
 </sst>
 </file>
@@ -405,13 +402,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -448,26 +448,17 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{EB3C8E1F-2402-4181-BF37-725B82379558}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{0E57637F-5B28-4293-BD68-4B33709FE286}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>